<commit_message>
Agregando las energías producidas
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="16">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -43,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="141">
+  <borders count="154">
     <border>
       <left/>
       <right/>
@@ -191,11 +230,24 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -337,6 +389,19 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,121 +419,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>2</v>
-      </c>
-    </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando baterias, quedó error
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="20">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -82,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="154">
+  <borders count="158">
     <border>
       <left/>
       <right/>
@@ -243,11 +255,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -402,6 +418,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +439,7 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="139" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Graficando las graficas de los equipos y lcoe
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -94,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="158">
+  <borders count="166">
     <border>
       <left/>
       <right/>
@@ -259,11 +283,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -422,6 +454,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +479,7 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="139" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Cambios lectura de los excel+graficos
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -118,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="166">
+  <borders count="171">
     <border>
       <left/>
       <right/>
@@ -291,11 +306,16 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -462,6 +482,11 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +504,7 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="139" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Quitando baterias del diagrama chart
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="35">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -133,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="223">
+  <borders count="225">
     <border>
       <left/>
       <right/>
@@ -363,11 +369,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -591,6 +599,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,121 +618,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="221" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios de titulos de graficos
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="35">
   <si>
     <t>horas</t>
   </si>
@@ -139,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="225">
+  <borders count="229">
     <border>
       <left/>
       <right/>
@@ -371,11 +371,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -601,6 +605,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,122 +625,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="221" t="s">
+      <c r="A3" s="227" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Seleccionando equipo más cercano al promedio
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -139,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="229">
+  <borders count="233">
     <border>
       <left/>
       <right/>
@@ -375,11 +387,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -609,6 +625,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,121 +646,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="227" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando energía diesel límitada
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="44">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -154,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="234">
+  <borders count="238">
     <border>
       <left/>
       <right/>
@@ -395,11 +407,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -634,6 +650,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,7 +671,7 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="227" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Modificando las graficas + área dependiente
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -166,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="250">
+  <borders count="259">
     <border>
       <left/>
       <right/>
@@ -423,11 +450,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="250">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -678,6 +714,15 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,121 +740,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="248" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Multiple energía + suave optimización
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -193,7 +217,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="263">
+  <borders count="271">
     <border>
       <left/>
       <right/>
@@ -463,11 +487,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="263">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -731,6 +763,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,121 +788,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="261" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglando el problema de las baterias
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -217,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="271">
+  <borders count="274">
     <border>
       <left/>
       <right/>
@@ -495,11 +504,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -771,6 +783,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,7 +803,7 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="261" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Comentando donde toca MIRAR
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="64">
   <si>
     <t>horas</t>
   </si>
@@ -226,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="274">
+  <borders count="276">
     <border>
       <left/>
       <right/>
@@ -507,11 +507,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -786,6 +788,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,122 +806,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="261" t="s">
+      <c r="A3" s="274" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New pie chart + prob mutar 1%
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -226,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="292">
+  <borders count="300">
     <border>
       <left/>
       <right/>
@@ -525,11 +549,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="292">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -822,6 +854,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,121 +879,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="290" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enviando los cambios del excel
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="72">
   <si>
     <t>horas</t>
   </si>
@@ -250,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="300">
+  <borders count="322">
     <border>
       <left/>
       <right/>
@@ -557,11 +557,33 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="300">
+  <cellXfs count="322">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -862,6 +884,28 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,122 +922,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="290" t="s">
+      <c r="A3" s="320" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios de los valores
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -250,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="322">
+  <borders count="326">
     <border>
       <left/>
       <right/>
@@ -579,11 +591,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="322">
+  <cellXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -906,6 +922,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,121 +943,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="320" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambio Valor Generador Diesel
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="76">
   <si>
     <t>horas</t>
   </si>
@@ -262,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="392">
+  <borders count="394">
     <border>
       <left/>
       <right/>
@@ -661,11 +661,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="392">
+  <cellXfs count="394">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1058,6 +1060,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,7 +1078,7 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="390" t="s">
+      <c r="A3" s="392" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglos grafica + revertir
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="85">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -283,7 +289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="413">
+  <borders count="415">
     <border>
       <left/>
       <right/>
@@ -703,11 +709,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="413">
+  <cellXfs count="415">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1121,6 +1129,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,121 +1148,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="411" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios configuracion generador diesel
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="87">
   <si>
     <t>horas</t>
   </si>
@@ -295,7 +295,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="417">
+  <borders count="479">
     <border>
       <left/>
       <right/>
@@ -719,11 +719,73 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="417">
+  <cellXfs count="479">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1141,6 +1203,68 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1157,122 +1281,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="411" t="s">
+      <c r="A3" s="477" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglando problema de parentesis
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="89">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -295,7 +301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="479">
+  <borders count="481">
     <border>
       <left/>
       <right/>
@@ -781,11 +787,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="479">
+  <cellXfs count="481">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1265,6 +1273,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,121 +1292,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="477" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando los demás archivos
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="89">
   <si>
     <t>horas</t>
   </si>
@@ -301,7 +301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="529">
+  <borders count="481">
     <border>
       <left/>
       <right/>
@@ -789,59 +789,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="529">
+  <cellXfs count="481">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1323,54 +1275,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="505" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="506" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="507" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="508" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="509" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="510" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="511" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="512" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="513" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="514" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="515" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="516" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="517" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="518" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="519" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="520" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="521" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="522" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="523" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="524" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="525" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="526" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="527" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="528" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1387,122 +1291,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="527" t="s">
+      <c r="A3" s="477" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cargando datos desde excel
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="92">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -301,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="531">
+  <borders count="534">
     <border>
       <left/>
       <right/>
@@ -839,11 +848,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="531">
+  <cellXfs count="534">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1375,6 +1387,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="528" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="529" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="530" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="531" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="532" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="533" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,121 +1407,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="529" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando las ecuaciones de turbina
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="94">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -310,7 +316,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="534">
+  <borders count="536">
     <border>
       <left/>
       <right/>
@@ -851,11 +857,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="534">
+  <cellXfs count="536">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1390,6 +1398,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="531" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="532" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="535" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1407,7 +1417,7 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="529" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Corrección variables + corrección guardar
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="98">
   <si>
     <t>horas</t>
   </si>
@@ -328,7 +328,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="540">
+  <borders count="568">
     <border>
       <left/>
       <right/>
@@ -875,11 +875,39 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="540">
+  <cellXfs count="568">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1420,6 +1448,34 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="537" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="538" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="539" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="544" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="545" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="546" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="551" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="552" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="553" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="558" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="559" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="560" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="565" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="566" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="567" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1436,122 +1492,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="529" t="s">
+      <c r="A3" s="566" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Guarda correctamente todos los datos
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="100">
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
   <si>
     <t>horas</t>
   </si>
@@ -328,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="616">
+  <borders count="618">
     <border>
       <left/>
       <right/>
@@ -951,11 +957,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="616">
+  <cellXfs count="618">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1572,6 +1580,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="613" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="614" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="615" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="616" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="617" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1589,121 +1599,121 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="614" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios en la interfaz app1
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="100">
   <si>
     <t>horas</t>
   </si>
@@ -334,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="618">
+  <borders count="634">
     <border>
       <left/>
       <right/>
@@ -959,11 +959,27 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="618">
+  <cellXfs count="634">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1582,6 +1598,22 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="615" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="616" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="621" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="622" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="623" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="628" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="629" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="630" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="633" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1598,122 +1630,122 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="614" t="s">
+      <c r="A3" s="632" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios LCOE de cada tecnologia
</commit_message>
<xml_diff>
--- a/test_curva_carga.xlsx
+++ b/test_curva_carga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="100">
   <si>
     <t>horas</t>
   </si>
@@ -334,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="668">
+  <borders count="682">
     <border>
       <left/>
       <right/>
@@ -1009,11 +1009,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="668">
+  <cellXfs count="682">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1682,6 +1696,20 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="665" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="666" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="670" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="671" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="672" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="673" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="674" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="675" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="676" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="677" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="678" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="679" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="680" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="681" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,7 +1726,7 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="666" t="s">
+      <c r="A3" s="680" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>